<commit_message>
add values for RCL of paraiba in 2014
</commit_message>
<xml_diff>
--- a/data-raw/RCL_CAMBIO_IPV_IBC_IGPDI_BRASIL Patricia_Luciano.xlsx
+++ b/data-raw/RCL_CAMBIO_IPV_IBC_IGPDI_BRASIL Patricia_Luciano.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="25317"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15480" windowHeight="7155" tabRatio="658" activeTab="10"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15480" windowHeight="7160" tabRatio="658" firstSheet="14" activeTab="25"/>
   </bookViews>
   <sheets>
     <sheet name="ES" sheetId="28" r:id="rId1"/>
@@ -35,7 +35,12 @@
     <sheet name="PB" sheetId="23" r:id="rId26"/>
     <sheet name="AL" sheetId="24" r:id="rId27"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -195,13 +200,13 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="0.00_ ;\-0.00\ "/>
-    <numFmt numFmtId="167" formatCode="0.0"/>
+    <numFmt numFmtId="166" formatCode="0.0"/>
   </numFmts>
-  <fonts count="35">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -250,28 +255,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -288,28 +272,6 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -355,6 +317,7 @@
       <family val="2"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
       <color indexed="9"/>
       <name val="Calibri"/>
@@ -362,55 +325,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color indexed="20"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color indexed="52"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color indexed="9"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color indexed="23"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color indexed="17"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color indexed="56"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color indexed="56"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color indexed="56"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -433,21 +348,23 @@
       <family val="2"/>
     </font>
     <font>
-      <b/>
+      <u/>
       <sz val="11"/>
-      <color indexed="63"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color indexed="56"/>
-      <name val="Cambria"/>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="57">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -456,37 +373,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
       </patternFill>
     </fill>
     <fill>
@@ -629,97 +521,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="31"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="45"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor indexed="42"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="46"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="27"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor indexed="47"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="44"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="29"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="11"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="51"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="30"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="36"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="49"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="52"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="62"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="10"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="57"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="53"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="22"/>
       </patternFill>
     </fill>
     <fill>
@@ -750,7 +557,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="18">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -818,45 +625,6 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -899,33 +667,6 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="thick">
-        <color indexed="62"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thick">
-        <color indexed="22"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="30"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
       <bottom style="double">
         <color indexed="52"/>
       </bottom>
@@ -946,23 +687,8 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="63"/>
-      </left>
-      <right style="thin">
-        <color indexed="63"/>
-      </right>
-      <top style="thin">
-        <color indexed="63"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="63"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="85">
+  <cellStyleXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -970,189 +696,113 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="15" fillId="30" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="29" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="32" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="42" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="43" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="44" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="45" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="46" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="47" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="48" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="49" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="44" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="45" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="50" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="51" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="52" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="26" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="38" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="32" fillId="53" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="54" borderId="16" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="33" fillId="51" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="55" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="35"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="17" fontId="0" fillId="55" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="55" borderId="0" xfId="84" applyFont="1" applyFill="1"/>
-    <xf numFmtId="4" fontId="0" fillId="55" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="17" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="33" borderId="0" xfId="46" applyFont="1" applyFill="1"/>
+    <xf numFmtId="4" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="55" borderId="0" xfId="84" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="0" fillId="55" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="33" borderId="0" xfId="46" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="0" fillId="56" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="167" fontId="0" fillId="55" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="0" fillId="55" borderId="0" xfId="84" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="33" borderId="0" xfId="46" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="85">
-    <cellStyle name="20% - Accent1" xfId="43"/>
-    <cellStyle name="20% - Accent2" xfId="44"/>
-    <cellStyle name="20% - Accent3" xfId="45"/>
-    <cellStyle name="20% - Accent4" xfId="46"/>
-    <cellStyle name="20% - Accent5" xfId="47"/>
-    <cellStyle name="20% - Accent6" xfId="48"/>
-    <cellStyle name="20% - Ênfase1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Ênfase2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Ênfase3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Ênfase4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Ênfase5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Ênfase6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Accent1" xfId="49"/>
-    <cellStyle name="40% - Accent2" xfId="50"/>
-    <cellStyle name="40% - Accent3" xfId="51"/>
-    <cellStyle name="40% - Accent4" xfId="52"/>
-    <cellStyle name="40% - Accent5" xfId="53"/>
-    <cellStyle name="40% - Accent6" xfId="54"/>
-    <cellStyle name="40% - Ênfase1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Ênfase2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Ênfase3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Ênfase4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Ênfase5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Ênfase6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Accent1" xfId="55"/>
-    <cellStyle name="60% - Accent2" xfId="56"/>
-    <cellStyle name="60% - Accent3" xfId="57"/>
-    <cellStyle name="60% - Accent4" xfId="58"/>
-    <cellStyle name="60% - Accent5" xfId="59"/>
-    <cellStyle name="60% - Accent6" xfId="60"/>
-    <cellStyle name="60% - Ênfase1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Ênfase2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Ênfase3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Ênfase4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Ênfase5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Ênfase6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Accent1" xfId="61"/>
-    <cellStyle name="Accent2" xfId="62"/>
-    <cellStyle name="Accent3" xfId="63"/>
-    <cellStyle name="Accent4" xfId="64"/>
-    <cellStyle name="Accent5" xfId="65"/>
-    <cellStyle name="Accent6" xfId="66"/>
-    <cellStyle name="Bad" xfId="67"/>
-    <cellStyle name="Bom" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Calculation" xfId="68"/>
-    <cellStyle name="Cálculo" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Célula de Verificação" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Célula Vinculada" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Check Cell" xfId="69"/>
-    <cellStyle name="Ênfase1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Ênfase2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Ênfase3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Ênfase4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Ênfase5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Ênfase6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Entrada" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Explanatory Text" xfId="70"/>
-    <cellStyle name="Good" xfId="71"/>
-    <cellStyle name="Heading 1" xfId="72"/>
-    <cellStyle name="Heading 2" xfId="73"/>
-    <cellStyle name="Heading 3" xfId="74"/>
-    <cellStyle name="Heading 4" xfId="75"/>
-    <cellStyle name="Incorreto" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Input" xfId="76"/>
-    <cellStyle name="Linked Cell" xfId="77"/>
-    <cellStyle name="Neutra" xfId="8" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="Neutral" xfId="78"/>
+  <cellStyles count="47">
+    <cellStyle name="20% - Accent1" xfId="12"/>
+    <cellStyle name="20% - Accent2" xfId="16"/>
+    <cellStyle name="20% - Accent3" xfId="20"/>
+    <cellStyle name="20% - Accent4" xfId="24"/>
+    <cellStyle name="20% - Accent5" xfId="28"/>
+    <cellStyle name="20% - Accent6" xfId="32"/>
+    <cellStyle name="40% - Accent1" xfId="13"/>
+    <cellStyle name="40% - Accent2" xfId="17"/>
+    <cellStyle name="40% - Accent3" xfId="21"/>
+    <cellStyle name="40% - Accent4" xfId="25"/>
+    <cellStyle name="40% - Accent5" xfId="29"/>
+    <cellStyle name="40% - Accent6" xfId="33"/>
+    <cellStyle name="60% - Accent1" xfId="14"/>
+    <cellStyle name="60% - Accent2" xfId="18"/>
+    <cellStyle name="60% - Accent3" xfId="22"/>
+    <cellStyle name="60% - Accent4" xfId="26"/>
+    <cellStyle name="60% - Accent5" xfId="30"/>
+    <cellStyle name="60% - Accent6" xfId="34"/>
+    <cellStyle name="Accent1" xfId="11"/>
+    <cellStyle name="Accent2" xfId="15"/>
+    <cellStyle name="Accent3" xfId="19"/>
+    <cellStyle name="Accent4" xfId="23"/>
+    <cellStyle name="Accent5" xfId="27"/>
+    <cellStyle name="Accent6" xfId="31"/>
+    <cellStyle name="Bad" xfId="6"/>
+    <cellStyle name="Calculation" xfId="8"/>
+    <cellStyle name="Check Cell" xfId="36" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Comma" xfId="46" builtinId="3"/>
+    <cellStyle name="Explanatory Text" xfId="9"/>
+    <cellStyle name="Followed Hyperlink" xfId="37" builtinId="9" hidden="1"/>
+    <cellStyle name="Good" xfId="38" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="2"/>
+    <cellStyle name="Heading 2" xfId="3"/>
+    <cellStyle name="Heading 3" xfId="4"/>
+    <cellStyle name="Heading 4" xfId="5"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Input" xfId="39" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="40" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Neutral" xfId="41" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="42"/>
-    <cellStyle name="Normal 2 2" xfId="83"/>
-    <cellStyle name="Nota" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Note" xfId="79"/>
-    <cellStyle name="Output" xfId="80"/>
-    <cellStyle name="Saída" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Separador de milhares" xfId="84" builtinId="3"/>
-    <cellStyle name="Texto de Aviso" xfId="14" builtinId="11" customBuiltin="1"/>
-    <cellStyle name="Texto Explicativo" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Title" xfId="81"/>
-    <cellStyle name="Título" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Título 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Título 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Título 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Título 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Warning Text" xfId="82"/>
+    <cellStyle name="Normal 2" xfId="35"/>
+    <cellStyle name="Normal 2 2" xfId="45"/>
+    <cellStyle name="Note" xfId="42" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="7"/>
+    <cellStyle name="Title" xfId="1"/>
+    <cellStyle name="Total" xfId="10" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="44" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1451,18 +1101,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B183"/>
   <sheetViews>
     <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1"/>
-    <col min="2" max="2" width="15.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="8.83203125" style="1"/>
+    <col min="2" max="2" width="15.5" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -2815,12 +2465,17 @@
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr enableFormatConditionsCalculation="0">
     <tabColor rgb="FF00B050"/>
   </sheetPr>
   <dimension ref="A1:F184"/>
@@ -2829,13 +2484,13 @@
       <selection activeCell="K194" sqref="K194"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="2"/>
-    <col min="2" max="2" width="15.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="9.140625" style="2"/>
-    <col min="5" max="5" width="8.5703125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="2"/>
+    <col min="1" max="1" width="8.83203125" style="2"/>
+    <col min="2" max="2" width="15.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="8.83203125" style="2"/>
+    <col min="5" max="5" width="8.5" style="2" customWidth="1"/>
+    <col min="6" max="6" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -6114,25 +5769,30 @@
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr enableFormatConditionsCalculation="0">
     <tabColor rgb="FF00B050"/>
   </sheetPr>
   <dimension ref="A1:F184"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A164" workbookViewId="0">
+    <sheetView topLeftCell="A159" workbookViewId="0">
       <selection activeCell="L182" sqref="L182"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="2"/>
-    <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="2"/>
+    <col min="1" max="1" width="8.83203125" style="2"/>
+    <col min="2" max="2" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -9534,12 +9194,17 @@
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr enableFormatConditionsCalculation="0">
     <tabColor rgb="FF00B050"/>
   </sheetPr>
   <dimension ref="A1:F184"/>
@@ -9548,10 +9213,10 @@
       <selection activeCell="B170" sqref="B170:B181"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="2"/>
+    <col min="2" max="2" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -12403,12 +12068,17 @@
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr enableFormatConditionsCalculation="0">
     <tabColor rgb="FF00B050"/>
   </sheetPr>
   <dimension ref="A1:F184"/>
@@ -12417,11 +12087,11 @@
       <selection activeCell="K181" sqref="K181"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="2"/>
-    <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="2"/>
+    <col min="1" max="1" width="8.83203125" style="2"/>
+    <col min="2" max="2" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -15823,12 +15493,17 @@
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr enableFormatConditionsCalculation="0">
     <tabColor rgb="FF00B050"/>
   </sheetPr>
   <dimension ref="A1:F184"/>
@@ -15837,11 +15512,11 @@
       <selection activeCell="B181" sqref="B38:B181"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="2"/>
-    <col min="2" max="2" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="9.140625" style="2"/>
+    <col min="1" max="1" width="8.83203125" style="2"/>
+    <col min="2" max="2" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -19243,22 +18918,27 @@
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F184"/>
   <sheetViews>
     <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="K28" sqref="K28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="2"/>
-    <col min="2" max="2" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="9.140625" style="2"/>
+    <col min="1" max="1" width="8.83203125" style="2"/>
+    <col min="2" max="2" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -22660,20 +22340,25 @@
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F184"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="2"/>
-    <col min="2" max="2" width="13.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="9.140625" style="2"/>
+    <col min="1" max="1" width="8.83203125" style="2"/>
+    <col min="2" max="2" width="13.83203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -26051,22 +25736,27 @@
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F184"/>
   <sheetViews>
     <sheetView topLeftCell="A169" workbookViewId="0">
       <selection activeCell="B38" sqref="B38:B181"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="2"/>
-    <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="9.140625" style="2"/>
+    <col min="1" max="1" width="8.83203125" style="2"/>
+    <col min="2" max="2" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -29468,20 +29158,25 @@
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G184"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="2"/>
-    <col min="2" max="2" width="13.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="9.140625" style="2"/>
+    <col min="1" max="1" width="8.83203125" style="2"/>
+    <col min="2" max="2" width="13.83203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -32814,21 +32509,26 @@
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F184"/>
   <sheetViews>
     <sheetView topLeftCell="A29" workbookViewId="0">
       <selection activeCell="H37" sqref="H37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="15.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="9.140625" style="2"/>
+    <col min="2" max="2" width="15.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -36232,12 +35932,17 @@
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr enableFormatConditionsCalculation="0">
     <tabColor rgb="FF00B050"/>
   </sheetPr>
   <dimension ref="A1:F183"/>
@@ -36246,13 +35951,13 @@
       <selection activeCell="B170" sqref="B170:B181"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1"/>
-    <col min="2" max="2" width="15.85546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="13.7109375" customWidth="1"/>
-    <col min="4" max="4" width="13.140625" customWidth="1"/>
-    <col min="5" max="5" width="8.5703125" customWidth="1"/>
+    <col min="1" max="1" width="8.83203125" style="1"/>
+    <col min="2" max="2" width="15.83203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" customWidth="1"/>
+    <col min="4" max="4" width="13.1640625" customWidth="1"/>
+    <col min="5" max="5" width="8.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -39562,12 +39267,17 @@
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr enableFormatConditionsCalculation="0">
     <tabColor rgb="FF00B0F0"/>
   </sheetPr>
   <dimension ref="A1:F184"/>
@@ -39576,11 +39286,11 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="2"/>
-    <col min="2" max="2" width="20.7109375" style="11" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="8.83203125" style="2"/>
+    <col min="2" max="2" width="20.6640625" style="11" customWidth="1"/>
+    <col min="3" max="16384" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -42898,12 +42608,17 @@
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr enableFormatConditionsCalculation="0">
     <tabColor rgb="FF00B0F0"/>
   </sheetPr>
   <dimension ref="A1:F184"/>
@@ -42912,11 +42627,11 @@
       <selection activeCell="R27" sqref="R27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="2"/>
-    <col min="2" max="2" width="20.7109375" style="11" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="8.83203125" style="2"/>
+    <col min="2" max="2" width="20.6640625" style="11" customWidth="1"/>
+    <col min="3" max="16384" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -46234,21 +45949,26 @@
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F184"/>
   <sheetViews>
     <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="15.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" style="2"/>
+    <col min="2" max="2" width="15.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -49097,12 +48817,17 @@
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr enableFormatConditionsCalculation="0">
     <tabColor rgb="FF00B0F0"/>
   </sheetPr>
   <dimension ref="A1:F184"/>
@@ -49111,11 +48836,11 @@
       <selection activeCell="Q79" sqref="Q79"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="2"/>
-    <col min="2" max="2" width="20.7109375" style="11" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="8.83203125" style="2"/>
+    <col min="2" max="2" width="20.6640625" style="11" customWidth="1"/>
+    <col min="3" max="16384" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -51881,12 +51606,17 @@
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr enableFormatConditionsCalculation="0">
     <tabColor rgb="FF00B0F0"/>
   </sheetPr>
   <dimension ref="A1:F184"/>
@@ -51895,11 +51625,11 @@
       <selection activeCell="M27" sqref="M27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="2"/>
-    <col min="2" max="2" width="20.7109375" style="11" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="8.83203125" style="2"/>
+    <col min="2" max="2" width="20.6640625" style="11" customWidth="1"/>
+    <col min="3" max="16384" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -54641,12 +54371,17 @@
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr enableFormatConditionsCalculation="0">
     <tabColor rgb="FF00B0F0"/>
   </sheetPr>
   <dimension ref="A1:F184"/>
@@ -54655,11 +54390,11 @@
       <selection activeCell="O50" sqref="O50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="2"/>
-    <col min="2" max="2" width="20.7109375" style="11" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="8.83203125" style="2"/>
+    <col min="2" max="2" width="20.6640625" style="11" customWidth="1"/>
+    <col min="3" max="16384" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -57425,25 +57160,30 @@
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr enableFormatConditionsCalculation="0">
     <tabColor rgb="FF00B0F0"/>
   </sheetPr>
   <dimension ref="A1:F184"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A160" workbookViewId="0">
+      <selection activeCell="B170" sqref="B170:B181"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="2"/>
-    <col min="2" max="2" width="20.7109375" style="10" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="8.83203125" style="2"/>
+    <col min="2" max="2" width="20.6640625" style="10" customWidth="1"/>
+    <col min="3" max="16384" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -59940,6 +59680,9 @@
       <c r="A170" s="4">
         <v>41640</v>
       </c>
+      <c r="B170" s="14">
+        <v>688492000</v>
+      </c>
       <c r="D170" s="2">
         <v>119.5</v>
       </c>
@@ -59954,6 +59697,9 @@
       <c r="A171" s="4">
         <v>41671</v>
       </c>
+      <c r="B171" s="14">
+        <v>724773000</v>
+      </c>
       <c r="D171" s="2">
         <v>103.9</v>
       </c>
@@ -59968,6 +59714,9 @@
       <c r="A172" s="4">
         <v>41699</v>
       </c>
+      <c r="B172" s="14">
+        <v>546815000</v>
+      </c>
       <c r="D172" s="2">
         <v>111.7</v>
       </c>
@@ -59982,6 +59731,9 @@
       <c r="A173" s="4">
         <v>41730</v>
       </c>
+      <c r="B173" s="14">
+        <v>587357000</v>
+      </c>
       <c r="D173" s="2">
         <v>116</v>
       </c>
@@ -59996,6 +59748,9 @@
       <c r="A174" s="4">
         <v>41760</v>
       </c>
+      <c r="B174" s="14">
+        <v>735825000</v>
+      </c>
       <c r="D174" s="2">
         <v>125.2</v>
       </c>
@@ -60010,6 +59765,9 @@
       <c r="A175" s="4">
         <v>41791</v>
       </c>
+      <c r="B175" s="14">
+        <v>584814000</v>
+      </c>
       <c r="D175" s="2">
         <v>120.6</v>
       </c>
@@ -60024,6 +59782,9 @@
       <c r="A176" s="4">
         <v>41821</v>
       </c>
+      <c r="B176" s="14">
+        <v>544003000</v>
+      </c>
       <c r="D176" s="2">
         <v>117.3</v>
       </c>
@@ -60038,6 +59799,9 @@
       <c r="A177" s="4">
         <v>41852</v>
       </c>
+      <c r="B177" s="14">
+        <v>584080000</v>
+      </c>
       <c r="D177" s="2">
         <v>120.4</v>
       </c>
@@ -60052,6 +59816,9 @@
       <c r="A178" s="4">
         <v>41883</v>
       </c>
+      <c r="B178" s="14">
+        <v>577811000</v>
+      </c>
       <c r="D178" s="2">
         <v>119.5</v>
       </c>
@@ -60066,6 +59833,9 @@
       <c r="A179" s="4">
         <v>41913</v>
       </c>
+      <c r="B179" s="14">
+        <v>547983000</v>
+      </c>
       <c r="D179" s="2">
         <v>131.6</v>
       </c>
@@ -60080,6 +59850,9 @@
       <c r="A180" s="4">
         <v>41944</v>
       </c>
+      <c r="B180" s="14">
+        <v>607405000</v>
+      </c>
       <c r="D180" s="2">
         <v>134.9</v>
       </c>
@@ -60094,6 +59867,9 @@
       <c r="A181" s="4">
         <v>41974</v>
       </c>
+      <c r="B181" s="14">
+        <v>670431000</v>
+      </c>
       <c r="D181" s="2">
         <v>152.9</v>
       </c>
@@ -60134,12 +59910,18 @@
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr enableFormatConditionsCalculation="0">
     <tabColor rgb="FF00B0F0"/>
   </sheetPr>
   <dimension ref="A1:F184"/>
@@ -60148,11 +59930,11 @@
       <selection activeCell="O28" sqref="O28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="2"/>
-    <col min="2" max="2" width="20.7109375" style="11" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="8.83203125" style="2"/>
+    <col min="2" max="2" width="20.6640625" style="11" customWidth="1"/>
+    <col min="3" max="16384" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -62918,22 +62700,27 @@
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F184"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="2"/>
-    <col min="2" max="2" width="16.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="9.140625" style="2"/>
-    <col min="5" max="5" width="8.5703125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="2"/>
+    <col min="1" max="1" width="8.83203125" style="2"/>
+    <col min="2" max="2" width="16.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="8.83203125" style="2"/>
+    <col min="5" max="5" width="8.5" style="2" customWidth="1"/>
+    <col min="6" max="6" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -66212,22 +65999,27 @@
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F184"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="2"/>
-    <col min="2" max="2" width="16.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="9.140625" style="2"/>
-    <col min="5" max="5" width="8.5703125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="2"/>
+    <col min="1" max="1" width="8.83203125" style="2"/>
+    <col min="2" max="2" width="16.5" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="8.83203125" style="2"/>
+    <col min="5" max="5" width="8.5" style="2" customWidth="1"/>
+    <col min="6" max="6" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -69506,22 +69298,27 @@
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F184"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="2"/>
-    <col min="2" max="2" width="16.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="9.140625" style="2"/>
-    <col min="5" max="5" width="8.5703125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="2"/>
+    <col min="1" max="1" width="8.83203125" style="2"/>
+    <col min="2" max="2" width="16.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="8.83203125" style="2"/>
+    <col min="5" max="5" width="8.5" style="2" customWidth="1"/>
+    <col min="6" max="6" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -72800,22 +72597,27 @@
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F184"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="2"/>
-    <col min="2" max="2" width="16.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="9.140625" style="2"/>
-    <col min="5" max="5" width="8.5703125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="2"/>
+    <col min="1" max="1" width="8.83203125" style="2"/>
+    <col min="2" max="2" width="16.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="8.83203125" style="2"/>
+    <col min="5" max="5" width="8.5" style="2" customWidth="1"/>
+    <col min="6" max="6" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -76094,12 +75896,17 @@
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr enableFormatConditionsCalculation="0">
     <tabColor rgb="FF00B050"/>
   </sheetPr>
   <dimension ref="A1:F184"/>
@@ -76108,13 +75915,13 @@
       <selection activeCell="D190" sqref="D190"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="2"/>
-    <col min="2" max="2" width="15.28515625" style="1" customWidth="1"/>
-    <col min="3" max="4" width="9.140625" style="2"/>
-    <col min="5" max="5" width="8.5703125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="2"/>
+    <col min="1" max="1" width="8.83203125" style="2"/>
+    <col min="2" max="2" width="15.33203125" style="1" customWidth="1"/>
+    <col min="3" max="4" width="8.83203125" style="2"/>
+    <col min="5" max="5" width="8.5" style="2" customWidth="1"/>
+    <col min="6" max="6" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -79429,22 +79236,27 @@
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F184"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="2"/>
-    <col min="2" max="2" width="15.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="9.140625" style="2"/>
-    <col min="5" max="5" width="8.5703125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="2"/>
+    <col min="1" max="1" width="8.83203125" style="2"/>
+    <col min="2" max="2" width="15.5" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="8.83203125" style="2"/>
+    <col min="5" max="5" width="8.5" style="2" customWidth="1"/>
+    <col min="6" max="6" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -82723,22 +82535,27 @@
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F184"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="2"/>
-    <col min="2" max="2" width="15.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="9.140625" style="2"/>
-    <col min="5" max="5" width="8.5703125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="2"/>
+    <col min="1" max="1" width="8.83203125" style="2"/>
+    <col min="2" max="2" width="15.5" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="8.83203125" style="2"/>
+    <col min="5" max="5" width="8.5" style="2" customWidth="1"/>
+    <col min="6" max="6" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -86017,5 +85834,10 @@
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Altera rcl do sergipe pois estava igual a de tocantins
</commit_message>
<xml_diff>
--- a/data-raw/RCL_CAMBIO_IPV_IBC_IGPDI_BRASIL Patricia_Luciano.xlsx
+++ b/data-raw/RCL_CAMBIO_IPV_IBC_IGPDI_BRASIL Patricia_Luciano.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="25317"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="26221"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15480" windowHeight="7160" tabRatio="658" firstSheet="14" activeTab="25"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15460" tabRatio="658" firstSheet="14" activeTab="21"/>
   </bookViews>
   <sheets>
     <sheet name="ES" sheetId="28" r:id="rId1"/>
@@ -202,9 +202,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="3">
-    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="0.00_ ;\-0.00\ "/>
-    <numFmt numFmtId="166" formatCode="0.0"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="0.00_ ;\-0.00\ "/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
   <fonts count="22" x14ac:knownFonts="1">
     <font>
@@ -735,7 +735,7 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -744,14 +744,14 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="35"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="17" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="33" borderId="0" xfId="46" applyFont="1" applyFill="1"/>
+    <xf numFmtId="43" fontId="0" fillId="33" borderId="0" xfId="46" applyFont="1" applyFill="1"/>
     <xf numFmtId="4" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="33" borderId="0" xfId="46" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="33" borderId="0" xfId="46" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="166" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="33" borderId="0" xfId="46" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
@@ -45961,8 +45961,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F184"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B38" sqref="B38:B181"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -46387,7 +46387,7 @@
         <v>37622</v>
       </c>
       <c r="B38" s="6">
-        <v>127012000</v>
+        <v>146475413.15000001</v>
       </c>
       <c r="D38" s="2">
         <v>47.82</v>
@@ -46400,7 +46400,7 @@
         <v>37653</v>
       </c>
       <c r="B39" s="6">
-        <v>142374000</v>
+        <v>152839148.44</v>
       </c>
       <c r="D39" s="2">
         <v>45.09</v>
@@ -46413,7 +46413,7 @@
         <v>37681</v>
       </c>
       <c r="B40" s="6">
-        <v>122139000</v>
+        <v>144901570.37</v>
       </c>
       <c r="D40" s="2">
         <v>42.72</v>
@@ -46426,7 +46426,7 @@
         <v>37712</v>
       </c>
       <c r="B41" s="6">
-        <v>114437000</v>
+        <v>143172278.74000001</v>
       </c>
       <c r="D41" s="2">
         <v>45.1</v>
@@ -46439,7 +46439,7 @@
         <v>37742</v>
       </c>
       <c r="B42" s="6">
-        <v>149389000</v>
+        <v>172791273.02000001</v>
       </c>
       <c r="D42" s="2">
         <v>45.16</v>
@@ -46452,7 +46452,7 @@
         <v>37773</v>
       </c>
       <c r="B43" s="6">
-        <v>117328000</v>
+        <v>138187417.21000001</v>
       </c>
       <c r="D43" s="2">
         <v>43.78</v>
@@ -46465,7 +46465,7 @@
         <v>37803</v>
       </c>
       <c r="B44" s="6">
-        <v>107804000</v>
+        <v>128676875.06999999</v>
       </c>
       <c r="D44" s="2">
         <v>45.96</v>
@@ -46478,7 +46478,7 @@
         <v>37834</v>
       </c>
       <c r="B45" s="6">
-        <v>128909000</v>
+        <v>146532031.93000001</v>
       </c>
       <c r="D45" s="2">
         <v>46.88</v>
@@ -46491,7 +46491,7 @@
         <v>37865</v>
       </c>
       <c r="B46" s="6">
-        <v>117697000</v>
+        <v>147455782.36000001</v>
       </c>
       <c r="D46" s="2">
         <v>44</v>
@@ -46504,7 +46504,7 @@
         <v>37895</v>
       </c>
       <c r="B47" s="6">
-        <v>125859000</v>
+        <v>151577008.47999999</v>
       </c>
       <c r="D47" s="2">
         <v>47.62</v>
@@ -46517,7 +46517,7 @@
         <v>37926</v>
       </c>
       <c r="B48" s="6">
-        <v>138848000</v>
+        <v>159704359.80000001</v>
       </c>
       <c r="D48" s="2">
         <v>49.77</v>
@@ -46530,7 +46530,7 @@
         <v>37956</v>
       </c>
       <c r="B49" s="6">
-        <v>146137000</v>
+        <v>173154203.88999999</v>
       </c>
       <c r="D49" s="2">
         <v>68.48</v>
@@ -46545,7 +46545,7 @@
         <v>37987</v>
       </c>
       <c r="B50" s="6">
-        <v>142248000</v>
+        <v>173827051.12</v>
       </c>
       <c r="D50" s="2">
         <v>49.77</v>
@@ -46562,7 +46562,7 @@
         <v>38018</v>
       </c>
       <c r="B51" s="6">
-        <v>126145000</v>
+        <v>143876267.72</v>
       </c>
       <c r="D51" s="2">
         <v>45.48</v>
@@ -46579,7 +46579,7 @@
         <v>38047</v>
       </c>
       <c r="B52" s="6">
-        <v>134354000</v>
+        <v>178105432.84999999</v>
       </c>
       <c r="D52" s="2">
         <v>48.13</v>
@@ -46596,7 +46596,7 @@
         <v>38078</v>
       </c>
       <c r="B53" s="6">
-        <v>141793000</v>
+        <v>174143912.83000001</v>
       </c>
       <c r="D53" s="2">
         <v>47.06</v>
@@ -46613,7 +46613,7 @@
         <v>38108</v>
       </c>
       <c r="B54" s="6">
-        <v>160354000</v>
+        <v>176067903.84999999</v>
       </c>
       <c r="D54" s="2">
         <v>50.9</v>
@@ -46630,7 +46630,7 @@
         <v>38139</v>
       </c>
       <c r="B55" s="6">
-        <v>130170000</v>
+        <v>150487816.41</v>
       </c>
       <c r="D55" s="2">
         <v>49.67</v>
@@ -46647,7 +46647,7 @@
         <v>38169</v>
       </c>
       <c r="B56" s="6">
-        <v>141160000</v>
+        <v>152704035.50999999</v>
       </c>
       <c r="D56" s="2">
         <v>49.45</v>
@@ -46664,7 +46664,7 @@
         <v>38200</v>
       </c>
       <c r="B57" s="6">
-        <v>152031000</v>
+        <v>167268305.74000001</v>
       </c>
       <c r="D57" s="2">
         <v>49.5</v>
@@ -46681,7 +46681,7 @@
         <v>38231</v>
       </c>
       <c r="B58" s="6">
-        <v>138128000</v>
+        <v>173290098.49000001</v>
       </c>
       <c r="D58" s="2">
         <v>46.76</v>
@@ -46698,7 +46698,7 @@
         <v>38261</v>
       </c>
       <c r="B59" s="6">
-        <v>152300000</v>
+        <v>169903064.37</v>
       </c>
       <c r="D59" s="2">
         <v>49.48</v>
@@ -46715,7 +46715,7 @@
         <v>38292</v>
       </c>
       <c r="B60" s="6">
-        <v>141622000</v>
+        <v>167954488.88</v>
       </c>
       <c r="D60" s="2">
         <v>49.82</v>
@@ -46732,7 +46732,7 @@
         <v>38322</v>
       </c>
       <c r="B61" s="6">
-        <v>182806000</v>
+        <v>215478860.13</v>
       </c>
       <c r="D61" s="2">
         <v>71.98</v>
@@ -46749,7 +46749,7 @@
         <v>38353</v>
       </c>
       <c r="B62" s="6">
-        <v>196067166.44999999</v>
+        <v>217070676.75</v>
       </c>
       <c r="D62" s="2">
         <v>51.17</v>
@@ -46766,7 +46766,7 @@
         <v>38384</v>
       </c>
       <c r="B63" s="6">
-        <v>162099185.09</v>
+        <v>183529261.74000001</v>
       </c>
       <c r="D63" s="2">
         <v>55.71</v>
@@ -46783,7 +46783,7 @@
         <v>38412</v>
       </c>
       <c r="B64" s="6">
-        <v>159679146.68000001</v>
+        <v>185145883.21000001</v>
       </c>
       <c r="D64" s="2">
         <v>60.44</v>
@@ -46800,7 +46800,7 @@
         <v>38443</v>
       </c>
       <c r="B65" s="6">
-        <v>177702114.33000001</v>
+        <v>195901879.31</v>
       </c>
       <c r="D65" s="2">
         <v>58.55</v>
@@ -46817,7 +46817,7 @@
         <v>38473</v>
       </c>
       <c r="B66" s="6">
-        <v>187594028.38999999</v>
+        <v>222151844.61000001</v>
       </c>
       <c r="D66" s="2">
         <v>63.8</v>
@@ -46834,7 +46834,7 @@
         <v>38504</v>
       </c>
       <c r="B67" s="6">
-        <v>190580728.06999999</v>
+        <v>206754273.62</v>
       </c>
       <c r="D67" s="2">
         <v>63.71</v>
@@ -46851,7 +46851,7 @@
         <v>38534</v>
       </c>
       <c r="B68" s="6">
-        <v>175441607.25999999</v>
+        <v>212187409.87</v>
       </c>
       <c r="D68" s="2">
         <v>60.7</v>
@@ -46868,7 +46868,7 @@
         <v>38565</v>
       </c>
       <c r="B69" s="6">
-        <v>178180703.56</v>
+        <v>203525699.78</v>
       </c>
       <c r="D69" s="2">
         <v>64.260000000000005</v>
@@ -46885,7 +46885,7 @@
         <v>38596</v>
       </c>
       <c r="B70" s="6">
-        <v>157061229.88999999</v>
+        <v>177984558.94999999</v>
       </c>
       <c r="D70" s="2">
         <v>60.96</v>
@@ -46902,7 +46902,7 @@
         <v>38626</v>
       </c>
       <c r="B71" s="6">
-        <v>174002007.15000001</v>
+        <v>197437865.30000001</v>
       </c>
       <c r="D71" s="2">
         <v>72.14</v>
@@ -46919,7 +46919,7 @@
         <v>38657</v>
       </c>
       <c r="B72" s="6">
-        <v>185548344.21000001</v>
+        <v>223499581.34</v>
       </c>
       <c r="D72" s="2">
         <v>68.81</v>
@@ -46936,7 +46936,7 @@
         <v>38687</v>
       </c>
       <c r="B73" s="6">
-        <v>324453465.51999998</v>
+        <v>311468663.08999997</v>
       </c>
       <c r="D73" s="2">
         <v>99.43</v>
@@ -46953,7 +46953,7 @@
         <v>38718</v>
       </c>
       <c r="B74" s="6">
-        <v>143309154.53999999</v>
+        <v>232090350.30000001</v>
       </c>
       <c r="D74" s="2">
         <v>71.2</v>
@@ -46970,7 +46970,7 @@
         <v>38749</v>
       </c>
       <c r="B75" s="6">
-        <v>182207224.78</v>
+        <v>209461710.05000001</v>
       </c>
       <c r="D75" s="2">
         <v>54.71</v>
@@ -46987,7 +46987,7 @@
         <v>38777</v>
       </c>
       <c r="B76" s="6">
-        <v>178602552.34</v>
+        <v>211596183.38</v>
       </c>
       <c r="D76" s="2">
         <v>60.78</v>
@@ -47004,7 +47004,7 @@
         <v>38808</v>
       </c>
       <c r="B77" s="6">
-        <v>194778130.47</v>
+        <v>224186637.96000001</v>
       </c>
       <c r="D77" s="2">
         <v>59.01</v>
@@ -47021,7 +47021,7 @@
         <v>38838</v>
       </c>
       <c r="B78" s="6">
-        <v>208065714.69</v>
+        <v>242785929.71000001</v>
       </c>
       <c r="D78" s="2">
         <v>66.680000000000007</v>
@@ -47038,7 +47038,7 @@
         <v>38869</v>
       </c>
       <c r="B79" s="6">
-        <v>204692066.87</v>
+        <v>230630213.66</v>
       </c>
       <c r="D79" s="2">
         <v>63.49</v>
@@ -47055,7 +47055,7 @@
         <v>38899</v>
       </c>
       <c r="B80" s="6">
-        <v>201668221.27000001</v>
+        <v>259571313.00999999</v>
       </c>
       <c r="D80" s="2">
         <v>64.53</v>
@@ -47072,7 +47072,7 @@
         <v>38930</v>
       </c>
       <c r="B81" s="6">
-        <v>192418799.96000001</v>
+        <v>221806526.99000001</v>
       </c>
       <c r="D81" s="2">
         <v>69.62</v>
@@ -47089,7 +47089,7 @@
         <v>38961</v>
       </c>
       <c r="B82" s="6">
-        <v>191655140.72999999</v>
+        <v>224424393.87</v>
       </c>
       <c r="D82" s="2">
         <v>67.900000000000006</v>
@@ -47106,7 +47106,7 @@
         <v>38991</v>
       </c>
       <c r="B83" s="6">
-        <v>179819006.09999999</v>
+        <v>268776241.83999997</v>
       </c>
       <c r="D83" s="2">
         <v>69.75</v>
@@ -47123,7 +47123,7 @@
         <v>39022</v>
       </c>
       <c r="B84" s="6">
-        <v>207718541.88</v>
+        <v>256352609.44999999</v>
       </c>
       <c r="D84" s="2">
         <v>71.989999999999995</v>
@@ -47140,7 +47140,7 @@
         <v>39052</v>
       </c>
       <c r="B85" s="6">
-        <v>331486343</v>
+        <v>283992190.63</v>
       </c>
       <c r="D85" s="2">
         <v>97.64</v>
@@ -47157,7 +47157,7 @@
         <v>39083</v>
       </c>
       <c r="B86" s="6">
-        <v>144289393.30000001</v>
+        <v>248917068.69999999</v>
       </c>
       <c r="D86" s="2">
         <v>74.55</v>
@@ -47174,7 +47174,7 @@
         <v>39114</v>
       </c>
       <c r="B87" s="6">
-        <v>212577486.05000001</v>
+        <v>250128441.38999999</v>
       </c>
       <c r="D87" s="2">
         <v>64.25</v>
@@ -47191,7 +47191,7 @@
         <v>39142</v>
       </c>
       <c r="B88" s="6">
-        <v>194461547.34</v>
+        <v>216127119.78999999</v>
       </c>
       <c r="D88" s="2">
         <v>72.44</v>
@@ -47208,7 +47208,7 @@
         <v>39173</v>
       </c>
       <c r="B89" s="6">
-        <v>235558211.68000001</v>
+        <v>257438088.19999999</v>
       </c>
       <c r="D89" s="2">
         <v>66.69</v>
@@ -47225,7 +47225,7 @@
         <v>39203</v>
       </c>
       <c r="B90" s="6">
-        <v>256902836.13999999</v>
+        <v>251576647.75999999</v>
       </c>
       <c r="D90" s="2">
         <v>77.260000000000005</v>
@@ -47242,7 +47242,7 @@
         <v>39234</v>
       </c>
       <c r="B91" s="6">
-        <v>240436038.33000001</v>
+        <v>259883427.71000001</v>
       </c>
       <c r="D91" s="2">
         <v>73.52</v>
@@ -47259,7 +47259,7 @@
         <v>39264</v>
       </c>
       <c r="B92" s="6">
-        <v>223531467.19999999</v>
+        <v>233043477.50999999</v>
       </c>
       <c r="D92" s="2">
         <v>70.78</v>
@@ -47276,7 +47276,7 @@
         <v>39295</v>
       </c>
       <c r="B93" s="6">
-        <v>217241267.28</v>
+        <v>241434396.31</v>
       </c>
       <c r="D93" s="2">
         <v>75.36</v>
@@ -47293,7 +47293,7 @@
         <v>39326</v>
       </c>
       <c r="B94" s="6">
-        <v>239767639.37</v>
+        <v>247788825.24000001</v>
       </c>
       <c r="D94" s="2">
         <v>69.5</v>
@@ -47310,7 +47310,7 @@
         <v>39356</v>
       </c>
       <c r="B95" s="6">
-        <v>247813631.30000001</v>
+        <v>259706295.12</v>
       </c>
       <c r="D95" s="2">
         <v>73.11</v>
@@ -47327,7 +47327,7 @@
         <v>39387</v>
       </c>
       <c r="B96" s="6">
-        <v>271107655.42000002</v>
+        <v>274917180.10000002</v>
       </c>
       <c r="D96" s="2">
         <v>75.680000000000007</v>
@@ -47344,7 +47344,7 @@
         <v>39417</v>
       </c>
       <c r="B97" s="6">
-        <v>297762282.63</v>
+        <v>361927883.77999997</v>
       </c>
       <c r="D97" s="2">
         <v>104.41</v>
@@ -47361,7 +47361,7 @@
         <v>39448</v>
       </c>
       <c r="B98" s="6">
-        <v>271756722.31999999</v>
+        <v>330507838.91000003</v>
       </c>
       <c r="D98" s="2">
         <v>77.02</v>
@@ -47378,7 +47378,7 @@
         <v>39479</v>
       </c>
       <c r="B99" s="6">
-        <v>292263193.35000002</v>
+        <v>322098648.85000002</v>
       </c>
       <c r="D99" s="2">
         <v>68.27</v>
@@ -47395,7 +47395,7 @@
         <v>39508</v>
       </c>
       <c r="B100" s="6">
-        <v>243219387.84</v>
+        <v>270719301.30000001</v>
       </c>
       <c r="D100" s="2">
         <v>74.760000000000005</v>
@@ -47412,7 +47412,7 @@
         <v>39539</v>
       </c>
       <c r="B101" s="6">
-        <v>290418599.52999997</v>
+        <v>306346058.19999999</v>
       </c>
       <c r="D101" s="2">
         <v>70.61</v>
@@ -47429,7 +47429,7 @@
         <v>39569</v>
       </c>
       <c r="B102" s="6">
-        <v>300664012.33999997</v>
+        <v>305867302.19999999</v>
       </c>
       <c r="D102" s="2">
         <v>76.77</v>
@@ -47446,7 +47446,7 @@
         <v>39600</v>
       </c>
       <c r="B103" s="6">
-        <v>263978791.33000001</v>
+        <v>294497632.57999998</v>
       </c>
       <c r="D103" s="2">
         <v>72.209999999999994</v>
@@ -47463,7 +47463,7 @@
         <v>39630</v>
       </c>
       <c r="B104" s="6">
-        <v>256896846.43000001</v>
+        <v>302659720.26999998</v>
       </c>
       <c r="D104" s="2">
         <v>72.650000000000006</v>
@@ -47480,7 +47480,7 @@
         <v>39661</v>
       </c>
       <c r="B105" s="6">
-        <v>285133903.51999998</v>
+        <v>323043497.99000001</v>
       </c>
       <c r="D105" s="2">
         <v>75.62</v>
@@ -47497,7 +47497,7 @@
         <v>39692</v>
       </c>
       <c r="B106" s="6">
-        <v>266302613.18000001</v>
+        <v>314611482.51999998</v>
       </c>
       <c r="D106" s="2">
         <v>77.45</v>
@@ -47514,7 +47514,7 @@
         <v>39722</v>
       </c>
       <c r="B107" s="6">
-        <v>265264922.38999999</v>
+        <v>315828395.82999998</v>
       </c>
       <c r="D107" s="2">
         <v>81.87</v>
@@ -47531,7 +47531,7 @@
         <v>39753</v>
       </c>
       <c r="B108" s="6">
-        <v>306033896.88999999</v>
+        <v>342961967.30000001</v>
       </c>
       <c r="D108" s="2">
         <v>80.03</v>
@@ -47548,7 +47548,7 @@
         <v>39783</v>
       </c>
       <c r="B109" s="6">
-        <v>409074599.44999999</v>
+        <v>370622269.31</v>
       </c>
       <c r="D109" s="2">
         <v>107.37</v>
@@ -47565,7 +47565,7 @@
         <v>39814</v>
       </c>
       <c r="B110" s="6">
-        <v>212554870.87</v>
+        <v>345455769.99000001</v>
       </c>
       <c r="D110" s="2">
         <v>86.64</v>
@@ -47582,7 +47582,7 @@
         <v>39845</v>
       </c>
       <c r="B111" s="6">
-        <v>263080880.74000001</v>
+        <v>313551797.35000002</v>
       </c>
       <c r="D111" s="2">
         <v>73.58</v>
@@ -47599,7 +47599,7 @@
         <v>39873</v>
       </c>
       <c r="B112" s="6">
-        <v>246015748.69</v>
+        <v>274081087.56</v>
       </c>
       <c r="D112" s="2">
         <v>79.819999999999993</v>
@@ -47616,7 +47616,7 @@
         <v>39904</v>
       </c>
       <c r="B113" s="6">
-        <v>280394794.94999999</v>
+        <v>307116383.56999999</v>
       </c>
       <c r="D113" s="2">
         <v>79.56</v>
@@ -47633,7 +47633,7 @@
         <v>39934</v>
       </c>
       <c r="B114" s="6">
-        <v>333021332.63</v>
+        <v>328089111.24000001</v>
       </c>
       <c r="D114" s="2">
         <v>85.39</v>
@@ -47650,7 +47650,7 @@
         <v>39965</v>
       </c>
       <c r="B115" s="6">
-        <v>283996731.36000001</v>
+        <v>311711839.26999998</v>
       </c>
       <c r="D115" s="2">
         <v>83.45</v>
@@ -47667,7 +47667,7 @@
         <v>39995</v>
       </c>
       <c r="B116" s="6">
-        <v>257602229.34999999</v>
+        <v>293393052.51999998</v>
       </c>
       <c r="D116" s="2">
         <v>86.46</v>
@@ -47684,7 +47684,7 @@
         <v>40026</v>
       </c>
       <c r="B117" s="6">
-        <v>294984711.70999998</v>
+        <v>299122955.04000002</v>
       </c>
       <c r="D117" s="2">
         <v>88.77</v>
@@ -47701,7 +47701,7 @@
         <v>40057</v>
       </c>
       <c r="B118" s="6">
-        <v>262979155.94999999</v>
+        <v>299646479.5</v>
       </c>
       <c r="D118" s="2">
         <v>84.73</v>
@@ -47718,7 +47718,7 @@
         <v>40087</v>
       </c>
       <c r="B119" s="6">
-        <v>264149242.19</v>
+        <v>325457265.91000003</v>
       </c>
       <c r="D119" s="2">
         <v>92.54</v>
@@ -47735,7 +47735,7 @@
         <v>40118</v>
       </c>
       <c r="B120" s="6">
-        <v>332667918.04000002</v>
+        <v>363464054.70999998</v>
       </c>
       <c r="D120" s="2">
         <v>90.6</v>
@@ -47752,7 +47752,7 @@
         <v>40148</v>
       </c>
       <c r="B121" s="6">
-        <v>374968701.60000002</v>
+        <v>473175516.62</v>
       </c>
       <c r="D121" s="2">
         <v>126.26</v>
@@ -47769,7 +47769,7 @@
         <v>40179</v>
       </c>
       <c r="B122" s="6">
-        <v>287857358.13999999</v>
+        <v>352199076.41000003</v>
       </c>
       <c r="D122" s="2">
         <v>97.65</v>
@@ -47786,7 +47786,7 @@
         <v>40210</v>
       </c>
       <c r="B123" s="6">
-        <v>292046780.00999999</v>
+        <v>352081483.31999999</v>
       </c>
       <c r="D123" s="2">
         <v>87.29</v>
@@ -47803,7 +47803,7 @@
         <v>40238</v>
       </c>
       <c r="B124" s="6">
-        <v>281167466.22000003</v>
+        <v>318323098.00999999</v>
       </c>
       <c r="D124" s="2">
         <v>96</v>
@@ -47820,7 +47820,7 @@
         <v>40269</v>
       </c>
       <c r="B125" s="6">
-        <v>328766191.16000003</v>
+        <v>403334528.94999999</v>
       </c>
       <c r="D125" s="2">
         <v>88.21</v>
@@ -47837,7 +47837,7 @@
         <v>40299</v>
       </c>
       <c r="B126" s="6">
-        <v>329694894.75999999</v>
+        <v>436030063.55000001</v>
       </c>
       <c r="D126" s="2">
         <v>96.11</v>
@@ -47854,7 +47854,7 @@
         <v>40330</v>
       </c>
       <c r="B127" s="6">
-        <v>320550312.00999999</v>
+        <v>375372898.10000002</v>
       </c>
       <c r="D127" s="2">
         <v>94.21</v>
@@ -47871,7 +47871,7 @@
         <v>40360</v>
       </c>
       <c r="B128" s="6">
-        <v>326591024.77999997</v>
+        <v>338197522.41000003</v>
       </c>
       <c r="D128" s="2">
         <v>95.85</v>
@@ -47888,7 +47888,7 @@
         <v>40391</v>
       </c>
       <c r="B129" s="6">
-        <v>321334852.44999999</v>
+        <v>359171756.14999998</v>
       </c>
       <c r="D129" s="2">
         <v>97.6</v>
@@ -47905,7 +47905,7 @@
         <v>40422</v>
       </c>
       <c r="B130" s="6">
-        <v>310496475.32999998</v>
+        <v>374206733.24000001</v>
       </c>
       <c r="D130" s="2">
         <v>95.78</v>
@@ -47922,7 +47922,7 @@
         <v>40452</v>
       </c>
       <c r="B131" s="6">
-        <v>316652437.33999997</v>
+        <v>365799789.13</v>
       </c>
       <c r="D131" s="2">
         <v>102.16</v>
@@ -47939,7 +47939,7 @@
         <v>40483</v>
       </c>
       <c r="B132" s="6">
-        <v>331545188.80000001</v>
+        <v>426066748.38999999</v>
       </c>
       <c r="D132" s="2">
         <v>101.61</v>
@@ -47956,7 +47956,7 @@
         <v>40513</v>
       </c>
       <c r="B133" s="6">
-        <v>434526065.01999998</v>
+        <v>528603261.44</v>
       </c>
       <c r="D133" s="2">
         <v>141.49</v>
@@ -47973,7 +47973,7 @@
         <v>40544</v>
       </c>
       <c r="B134" s="6">
-        <v>375718784.75999999</v>
+        <v>448074546.06999999</v>
       </c>
       <c r="D134" s="2">
         <v>103.1</v>
@@ -47990,7 +47990,7 @@
         <v>40575</v>
       </c>
       <c r="B135" s="6">
-        <v>385998883.88</v>
+        <v>461058475.10000002</v>
       </c>
       <c r="D135" s="2">
         <v>87.84</v>
@@ -48007,7 +48007,7 @@
         <v>40603</v>
       </c>
       <c r="B136" s="6">
-        <v>314845525.79000002</v>
+        <v>375966953.39999998</v>
       </c>
       <c r="D136" s="2">
         <v>92.93</v>
@@ -48024,7 +48024,7 @@
         <v>40634</v>
       </c>
       <c r="B137" s="6">
-        <v>367537172.19</v>
+        <v>401531435.37</v>
       </c>
       <c r="D137" s="2">
         <v>93.47</v>
@@ -48041,7 +48041,7 @@
         <v>40664</v>
       </c>
       <c r="B138" s="6">
-        <v>406697469.32999998</v>
+        <v>403044267.08999997</v>
       </c>
       <c r="D138" s="2">
         <v>97.64</v>
@@ -48058,7 +48058,7 @@
         <v>40695</v>
       </c>
       <c r="B139" s="6">
-        <v>373088893.81</v>
+        <v>395371482.88</v>
       </c>
       <c r="D139" s="2">
         <v>95.78</v>
@@ -48075,7 +48075,7 @@
         <v>40725</v>
       </c>
       <c r="B140" s="6">
-        <v>351621769.93000001</v>
+        <v>372307514.10000002</v>
       </c>
       <c r="D140" s="2">
         <v>96.85</v>
@@ -48092,7 +48092,7 @@
         <v>40756</v>
       </c>
       <c r="B141" s="6">
-        <v>410269729.35000002</v>
+        <v>375669689.18000001</v>
       </c>
       <c r="D141" s="2">
         <v>98.57</v>
@@ -48109,7 +48109,7 @@
         <v>40787</v>
       </c>
       <c r="B142" s="6">
-        <v>314199679.52999997</v>
+        <v>345281540.11000001</v>
       </c>
       <c r="D142" s="2">
         <v>94.54</v>
@@ -48126,7 +48126,7 @@
         <v>40817</v>
       </c>
       <c r="B143" s="6">
-        <v>401921422.88999999</v>
+        <v>403812486.06</v>
       </c>
       <c r="D143" s="2">
         <v>99.85</v>
@@ -48143,7 +48143,7 @@
         <v>40848</v>
       </c>
       <c r="B144" s="6">
-        <v>382693587.58999997</v>
+        <v>447175062.43000001</v>
       </c>
       <c r="D144" s="2">
         <v>101.91</v>
@@ -48160,7 +48160,7 @@
         <v>40878</v>
       </c>
       <c r="B145" s="6">
-        <v>464202478.74000001</v>
+        <v>476294658.05000001</v>
       </c>
       <c r="D145" s="2">
         <v>137.52000000000001</v>
@@ -48177,7 +48177,7 @@
         <v>40909</v>
       </c>
       <c r="B146" s="6">
-        <v>408750558.48000002</v>
+        <v>426823395.01999998</v>
       </c>
       <c r="D146" s="2">
         <v>103.71</v>
@@ -48194,7 +48194,7 @@
         <v>40940</v>
       </c>
       <c r="B147" s="6">
-        <v>442661665.61000001</v>
+        <v>470346959.64999998</v>
       </c>
       <c r="D147" s="2">
         <v>96.8</v>
@@ -48211,7 +48211,7 @@
         <v>40969</v>
       </c>
       <c r="B148" s="6">
-        <v>363944466.69</v>
+        <v>383867796.86000001</v>
       </c>
       <c r="D148" s="2">
         <v>101.33</v>
@@ -48228,7 +48228,7 @@
         <v>41000</v>
       </c>
       <c r="B149" s="6">
-        <v>438118734.25</v>
+        <v>502438525.95999998</v>
       </c>
       <c r="D149" s="2">
         <v>96.47</v>
@@ -48245,7 +48245,7 @@
         <v>41030</v>
       </c>
       <c r="B150" s="6">
-        <v>420434956.94999999</v>
+        <v>474016798.12</v>
       </c>
       <c r="D150" s="2">
         <v>104.13</v>
@@ -48262,7 +48262,7 @@
         <v>41061</v>
       </c>
       <c r="B151" s="6">
-        <v>438382945.01999998</v>
+        <v>431078281.33999997</v>
       </c>
       <c r="D151" s="2">
         <v>100.74</v>
@@ -48279,7 +48279,7 @@
         <v>41091</v>
       </c>
       <c r="B152" s="6">
-        <v>386091758.31</v>
+        <v>395387052.22000003</v>
       </c>
       <c r="D152" s="2">
         <v>101.26</v>
@@ -48296,7 +48296,7 @@
         <v>41122</v>
       </c>
       <c r="B153" s="6">
-        <v>383444342.54000002</v>
+        <v>392642185.08999997</v>
       </c>
       <c r="D153" s="2">
         <v>105.3</v>
@@ -48313,7 +48313,7 @@
         <v>41153</v>
       </c>
       <c r="B154" s="6">
-        <v>354977351.76999998</v>
+        <v>381357900.79000002</v>
       </c>
       <c r="D154" s="2">
         <v>101.61</v>
@@ -48330,7 +48330,7 @@
         <v>41183</v>
       </c>
       <c r="B155" s="6">
-        <v>372560537.45999998</v>
+        <v>389410909.36000001</v>
       </c>
       <c r="D155" s="2">
         <v>106.15</v>
@@ -48347,7 +48347,7 @@
         <v>41214</v>
       </c>
       <c r="B156" s="6">
-        <v>427246596.55000001</v>
+        <v>453777610.25999999</v>
       </c>
       <c r="D156" s="2">
         <v>106.94</v>
@@ -48364,7 +48364,7 @@
         <v>41244</v>
       </c>
       <c r="B157" s="6">
-        <v>554861454.13</v>
+        <v>520507017.87</v>
       </c>
       <c r="D157" s="2">
         <v>140.69999999999999</v>
@@ -48381,7 +48381,7 @@
         <v>41275</v>
       </c>
       <c r="B158" s="6">
-        <v>418442435.36000001</v>
+        <v>472299304.23000002</v>
       </c>
       <c r="D158" s="2">
         <v>107.72</v>
@@ -48398,7 +48398,7 @@
         <v>41306</v>
       </c>
       <c r="B159" s="6">
-        <v>495318517.22000003</v>
+        <v>545498714.58000004</v>
       </c>
       <c r="D159" s="2">
         <v>94.88</v>
@@ -48415,7 +48415,7 @@
         <v>41334</v>
       </c>
       <c r="B160" s="6">
-        <v>352865262.12</v>
+        <v>396573882.5</v>
       </c>
       <c r="D160" s="2">
         <v>107.79</v>
@@ -48432,7 +48432,7 @@
         <v>41365</v>
       </c>
       <c r="B161" s="6">
-        <v>402637986.5</v>
+        <v>443413919.74000001</v>
       </c>
       <c r="D161" s="2">
         <v>100.79</v>
@@ -48449,7 +48449,7 @@
         <v>41395</v>
       </c>
       <c r="B162" s="6">
-        <v>480335641.25999999</v>
+        <v>508716451.88999999</v>
       </c>
       <c r="D162" s="2">
         <v>108.24</v>
@@ -48466,7 +48466,7 @@
         <v>41426</v>
       </c>
       <c r="B163" s="6">
-        <v>444583343.66000003</v>
+        <v>446639896.39999998</v>
       </c>
       <c r="D163" s="2">
         <v>102.88</v>
@@ -48483,7 +48483,7 @@
         <v>41456</v>
       </c>
       <c r="B164" s="6">
-        <v>403089182.14999998</v>
+        <v>395251304.99000001</v>
       </c>
       <c r="D164" s="2">
         <v>105.38</v>
@@ -48500,7 +48500,7 @@
         <v>41487</v>
       </c>
       <c r="B165" s="6">
-        <v>470784697.48000002</v>
+        <v>455078068.88999999</v>
       </c>
       <c r="D165" s="2">
         <v>110.61</v>
@@ -48517,7 +48517,7 @@
         <v>41518</v>
       </c>
       <c r="B166" s="6">
-        <v>402657843.42000002</v>
+        <v>413759547.10000002</v>
       </c>
       <c r="D166" s="2">
         <v>100.17</v>
@@ -48534,7 +48534,7 @@
         <v>41548</v>
       </c>
       <c r="B167" s="6">
-        <v>417983281.68000001</v>
+        <v>420006050.22000003</v>
       </c>
       <c r="D167" s="2">
         <v>110.36</v>
@@ -48551,7 +48551,7 @@
         <v>41579</v>
       </c>
       <c r="B168" s="6">
-        <v>491297809.74000001</v>
+        <v>503106109.04000002</v>
       </c>
       <c r="D168" s="2">
         <v>111.8</v>
@@ -48568,7 +48568,7 @@
         <v>41609</v>
       </c>
       <c r="B169" s="6">
-        <v>543444128.15999997</v>
+        <v>523931555.00999999</v>
       </c>
       <c r="D169" s="2">
         <v>140.4</v>
@@ -48585,7 +48585,7 @@
         <v>41640</v>
       </c>
       <c r="B170" s="6">
-        <v>518942014.19999999</v>
+        <v>570856604.17999995</v>
       </c>
       <c r="D170" s="2">
         <v>115.2</v>
@@ -48602,7 +48602,7 @@
         <v>41671</v>
       </c>
       <c r="B171" s="6">
-        <v>577131140.89999998</v>
+        <v>582933694.88999999</v>
       </c>
       <c r="D171" s="2">
         <v>101.4</v>
@@ -48619,7 +48619,7 @@
         <v>41699</v>
       </c>
       <c r="B172" s="6">
-        <v>419888901.23000002</v>
+        <v>434674925.68000001</v>
       </c>
       <c r="D172" s="2">
         <v>105.2</v>
@@ -48636,7 +48636,7 @@
         <v>41730</v>
       </c>
       <c r="B173" s="6">
-        <v>465970627.61000001</v>
+        <v>466732432.75</v>
       </c>
       <c r="D173" s="2">
         <v>103.3</v>
@@ -48653,7 +48653,7 @@
         <v>41760</v>
       </c>
       <c r="B174" s="6">
-        <v>601843752.20000005</v>
+        <v>525072922.32999998</v>
       </c>
       <c r="D174" s="2">
         <v>111.5</v>
@@ -48670,7 +48670,7 @@
         <v>41791</v>
       </c>
       <c r="B175" s="6">
-        <v>468965785.54000002</v>
+        <v>472716071.89999998</v>
       </c>
       <c r="D175" s="2">
         <v>100.5</v>
@@ -48687,7 +48687,7 @@
         <v>41821</v>
       </c>
       <c r="B176" s="6">
-        <v>455476544.81</v>
+        <v>441156193.94999999</v>
       </c>
       <c r="D176" s="2">
         <v>103</v>
@@ -48704,7 +48704,7 @@
         <v>41852</v>
       </c>
       <c r="B177" s="6">
-        <v>551491848.69000006</v>
+        <v>484929393.25999999</v>
       </c>
       <c r="D177" s="2">
         <v>108</v>
@@ -48721,7 +48721,7 @@
         <v>41883</v>
       </c>
       <c r="B178" s="6">
-        <v>450387225.55000001</v>
+        <v>443655970.38</v>
       </c>
       <c r="D178" s="2">
         <v>105.7</v>
@@ -48738,7 +48738,7 @@
         <v>41913</v>
       </c>
       <c r="B179" s="6">
-        <v>475891884.04000002</v>
+        <v>450217340.32999998</v>
       </c>
       <c r="D179" s="2">
         <v>110.5</v>
@@ -48755,7 +48755,7 @@
         <v>41944</v>
       </c>
       <c r="B180" s="6">
-        <v>530682400.37</v>
+        <v>529005871.36000001</v>
       </c>
       <c r="D180" s="2">
         <v>116.9</v>
@@ -48772,7 +48772,7 @@
         <v>41974</v>
       </c>
       <c r="B181" s="6">
-        <v>554778169.47000003</v>
+        <v>580533928.92999995</v>
       </c>
       <c r="D181" s="2">
         <v>141.1</v>
@@ -57175,7 +57175,7 @@
   </sheetPr>
   <dimension ref="A1:F184"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A160" workbookViewId="0">
+    <sheetView topLeftCell="A17" workbookViewId="0">
       <selection activeCell="B170" sqref="B170:B181"/>
     </sheetView>
   </sheetViews>

</xml_diff>